<commit_message>
added new venturi calculator
</commit_message>
<xml_diff>
--- a/8kN/analysis/Venturis/Venturi_Throat_Calculator.xlsx
+++ b/8kN/analysis/Venturis/Venturi_Throat_Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emilio\Documents\PSAS\liquid-propellant-engine\8kN\analysis\Venturis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A77319B4-AD71-420E-8715-FBF865C4820C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41047EB4-5409-4D65-90FB-9DF166F66272}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECDB9495-D873-43C0-B1A6-97F709E93988}"/>
   </bookViews>
@@ -131,10 +131,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -477,23 +477,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="13.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -511,97 +511,97 @@
         <v>0</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <v>2.1402999999999999</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <f>B4/(B5*SQRT(2*B6*(B7-B8)))</f>
         <v>2.5981307213825198E-5</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>0.94</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <f>2*SQRT(F4/PI())</f>
         <v>5.7515587251244504E-3</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <f>[1]!PropsSI("D","T",90.35,"P",B7,"OXYGEN")</f>
         <v>1147.4897022435114</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <f>F5*1000</f>
         <v>5.7515587251244504</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B7">
         <v>3356810.4856129801</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>10295.247479219748</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -621,96 +621,96 @@
         <v>0</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B12">
         <v>1.2157</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <f>B12/(B13*SQRT(2*B14*(B15-B16)))</f>
         <v>1.9095792398031301E-5</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>0.94</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <f>2*SQRT(F12/PI())</f>
         <v>4.9308739609958147E-3</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>785</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <f>F13*1000</f>
         <v>4.9308739609958145</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B15">
         <v>2926009.0739879799</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>4400</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>